<commit_message>
triangle_check, LCM Problem, String Task, contest Problem
</commit_message>
<xml_diff>
--- a/CP_Checklist.xlsx
+++ b/CP_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Coding\Competitive_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2897C8-0999-4AE9-A13B-2D2887FD4864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53074E2-2BCE-40EF-865A-CD9F39065606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13728" yWindow="0" windowWidth="9408" windowHeight="13056" xr2:uid="{87F4906E-34BE-4746-8434-6C162442B7FF}"/>
+    <workbookView xWindow="2196" yWindow="1308" windowWidth="9792" windowHeight="10692" xr2:uid="{87F4906E-34BE-4746-8434-6C162442B7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1495,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AD453A-40CD-4BCA-BF2D-B30251E79445}">
   <dimension ref="A1:A441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1640,12 +1640,12 @@
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1765,12 +1765,12 @@
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="9" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spiral traverse a matrix
</commit_message>
<xml_diff>
--- a/CP_Checklist.xlsx
+++ b/CP_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Coding\Competitive_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EB7469-5C59-4525-9370-B3A69E6AD7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F8991C-0E91-42E3-9D14-3069CDA94467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4056" yWindow="1248" windowWidth="9792" windowHeight="10692" xr2:uid="{87F4906E-34BE-4746-8434-6C162442B7FF}"/>
+    <workbookView xWindow="13728" yWindow="0" windowWidth="9408" windowHeight="13056" xr2:uid="{87F4906E-34BE-4746-8434-6C162442B7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1128,7 +1128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,12 +1144,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1195,7 +1189,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1520,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AD453A-40CD-4BCA-BF2D-B30251E79445}">
   <dimension ref="A1:A441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA58" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Patter of rhombus, where the n is at the centre and the border starts from 0
</commit_message>
<xml_diff>
--- a/CP_Checklist.xlsx
+++ b/CP_Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Coding\Competitive_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8FA872-23FE-4335-8C1C-4C4EAC0E35B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6EEE4E-45A9-4D72-BBF0-ADF7BE375797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{87F4906E-34BE-4746-8434-6C162442B7FF}"/>
   </bookViews>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AD453A-40CD-4BCA-BF2D-B30251E79445}">
   <dimension ref="A1:A441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="9" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>